<commit_message>
Add fallback and logging to missing panel downloader
Enhanced extra/missing.py to support fallback download URLs for missing panels, improved extension handling, added progress bar rendering, and implemented detailed logging of download attempts. New arguments allow specifying fallback templates and log file paths. Also added new image panels and updated missing reports.

as well as Added Chapter 3: panels 16 25 31
</commit_message>
<xml_diff>
--- a/reports/missing.xlsx
+++ b/reports/missing.xlsx
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C54" t="n">
         <v>1</v>
@@ -1500,11 +1500,7 @@
       <c r="D54" t="n">
         <v>24</v>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>2, 5, 13, 15</t>
-        </is>
-      </c>
+      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
@@ -1646,7 +1642,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C61" t="n">
         <v>1</v>
@@ -1654,11 +1650,7 @@
       <c r="D61" t="n">
         <v>20</v>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>9, 11, 18</t>
-        </is>
-      </c>
+      <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
@@ -1668,7 +1660,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C62" t="n">
         <v>2</v>
@@ -1676,11 +1668,7 @@
       <c r="D62" t="n">
         <v>18</v>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
@@ -1690,7 +1678,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C63" t="n">
         <v>1</v>
@@ -1698,11 +1686,7 @@
       <c r="D63" t="n">
         <v>21</v>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>5, 9, 12, 13, 14</t>
-        </is>
-      </c>
+      <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
@@ -1712,7 +1696,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C64" t="n">
         <v>1</v>
@@ -1720,11 +1704,7 @@
       <c r="D64" t="n">
         <v>22</v>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>7, 13, 15, 16, 19</t>
-        </is>
-      </c>
+      <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
     </row>
     <row r="65">
@@ -1734,7 +1714,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C65" t="n">
         <v>1</v>
@@ -1742,11 +1722,7 @@
       <c r="D65" t="n">
         <v>20</v>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>10, 17</t>
-        </is>
-      </c>
+      <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
     </row>
     <row r="66">
@@ -1756,7 +1732,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C66" t="n">
         <v>1</v>
@@ -1764,11 +1740,7 @@
       <c r="D66" t="n">
         <v>20</v>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>2, 8</t>
-        </is>
-      </c>
+      <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
@@ -1778,7 +1750,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C67" t="n">
         <v>1</v>
@@ -1786,11 +1758,7 @@
       <c r="D67" t="n">
         <v>20</v>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>14, 15</t>
-        </is>
-      </c>
+      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
     </row>
     <row r="68">
@@ -1800,7 +1768,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C68" t="n">
         <v>1</v>
@@ -1808,11 +1776,7 @@
       <c r="D68" t="n">
         <v>20</v>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
     </row>
     <row r="69">
@@ -1822,7 +1786,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C69" t="n">
         <v>1</v>
@@ -1830,11 +1794,7 @@
       <c r="D69" t="n">
         <v>20</v>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>4, 6, 16</t>
-        </is>
-      </c>
+      <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
     </row>
     <row r="70">
@@ -1844,7 +1804,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C70" t="n">
         <v>1</v>
@@ -1852,11 +1812,7 @@
       <c r="D70" t="n">
         <v>18</v>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>7, 13</t>
-        </is>
-      </c>
+      <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
     </row>
     <row r="71">
@@ -1866,7 +1822,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C71" t="n">
         <v>1</v>
@@ -1874,11 +1830,7 @@
       <c r="D71" t="n">
         <v>22</v>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
+      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
@@ -1888,7 +1840,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C72" t="n">
         <v>1</v>
@@ -1896,11 +1848,7 @@
       <c r="D72" t="n">
         <v>21</v>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>4, 8, 20</t>
-        </is>
-      </c>
+      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
     </row>
     <row r="73">
@@ -1910,7 +1858,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C73" t="n">
         <v>1</v>
@@ -1918,11 +1866,7 @@
       <c r="D73" t="n">
         <v>24</v>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>6, 7, 11, 20, 23</t>
-        </is>
-      </c>
+      <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
     </row>
     <row r="74">
@@ -1932,7 +1876,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C74" t="n">
         <v>1</v>
@@ -1940,11 +1884,7 @@
       <c r="D74" t="n">
         <v>23</v>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>6, 16</t>
-        </is>
-      </c>
+      <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
     </row>
     <row r="75">
@@ -1954,7 +1894,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C75" t="n">
         <v>1</v>
@@ -1962,11 +1902,7 @@
       <c r="D75" t="n">
         <v>20</v>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
+      <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
     </row>
     <row r="76">
@@ -1976,7 +1912,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C76" t="n">
         <v>1</v>
@@ -1984,11 +1920,7 @@
       <c r="D76" t="n">
         <v>20</v>
       </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>6, 7, 14</t>
-        </is>
-      </c>
+      <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
     </row>
     <row r="77">
@@ -1998,7 +1930,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C77" t="n">
         <v>1</v>
@@ -2006,11 +1938,7 @@
       <c r="D77" t="n">
         <v>22</v>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>6, 12, 16</t>
-        </is>
-      </c>
+      <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
     </row>
     <row r="78">
@@ -2020,7 +1948,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C78" t="n">
         <v>1</v>
@@ -2028,11 +1956,7 @@
       <c r="D78" t="n">
         <v>25</v>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>2, 17, 22</t>
-        </is>
-      </c>
+      <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
     </row>
     <row r="79">
@@ -2042,7 +1966,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C79" t="n">
         <v>2</v>
@@ -2050,11 +1974,7 @@
       <c r="D79" t="n">
         <v>22</v>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>5, 12, 20</t>
-        </is>
-      </c>
+      <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
     </row>
     <row r="80">
@@ -2064,7 +1984,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C80" t="n">
         <v>1</v>
@@ -2072,11 +1992,7 @@
       <c r="D80" t="n">
         <v>21</v>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>2, 8, 10, 15, 19</t>
-        </is>
-      </c>
+      <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
     </row>
     <row r="81">
@@ -2086,7 +2002,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C81" t="n">
         <v>2</v>
@@ -2094,11 +2010,7 @@
       <c r="D81" t="n">
         <v>23</v>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>8, 14, 18</t>
-        </is>
-      </c>
+      <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
     </row>
     <row r="82">
@@ -2108,7 +2020,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C82" t="n">
         <v>1</v>
@@ -2116,11 +2028,7 @@
       <c r="D82" t="n">
         <v>20</v>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
     </row>
     <row r="83">
@@ -2130,7 +2038,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C83" t="n">
         <v>1</v>
@@ -2138,11 +2046,7 @@
       <c r="D83" t="n">
         <v>22</v>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
     </row>
     <row r="84">
@@ -2152,7 +2056,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C84" t="n">
         <v>1</v>
@@ -2160,11 +2064,7 @@
       <c r="D84" t="n">
         <v>20</v>
       </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>2, 13, 19</t>
-        </is>
-      </c>
+      <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr"/>
     </row>
     <row r="85">
@@ -2174,7 +2074,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C85" t="n">
         <v>1</v>
@@ -2182,11 +2082,7 @@
       <c r="D85" t="n">
         <v>20</v>
       </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>9, 12, 13, 16</t>
-        </is>
-      </c>
+      <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
     </row>
     <row r="86">
@@ -2196,7 +2092,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C86" t="n">
         <v>1</v>
@@ -2204,11 +2100,7 @@
       <c r="D86" t="n">
         <v>20</v>
       </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>15, 17</t>
-        </is>
-      </c>
+      <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
     </row>
     <row r="87">
@@ -2218,7 +2110,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C87" t="n">
         <v>1</v>
@@ -2226,11 +2118,7 @@
       <c r="D87" t="n">
         <v>19</v>
       </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>2, 8, 14, 16</t>
-        </is>
-      </c>
+      <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
     </row>
     <row r="88">
@@ -2240,7 +2128,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C88" t="n">
         <v>2</v>
@@ -2248,11 +2136,7 @@
       <c r="D88" t="n">
         <v>20</v>
       </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>3, 12</t>
-        </is>
-      </c>
+      <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
     </row>
     <row r="89">
@@ -2262,7 +2146,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C89" t="n">
         <v>1</v>
@@ -2270,11 +2154,7 @@
       <c r="D89" t="n">
         <v>20</v>
       </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>5, 7, 9, 15</t>
-        </is>
-      </c>
+      <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
     </row>
     <row r="90">
@@ -2284,7 +2164,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C90" t="n">
         <v>1</v>
@@ -2292,11 +2172,7 @@
       <c r="D90" t="n">
         <v>22</v>
       </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>7, 10</t>
-        </is>
-      </c>
+      <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
     </row>
     <row r="91">
@@ -2306,7 +2182,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C91" t="n">
         <v>1</v>
@@ -2314,11 +2190,7 @@
       <c r="D91" t="n">
         <v>25</v>
       </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>7, 8, 16</t>
-        </is>
-      </c>
+      <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
     </row>
     <row r="92">
@@ -2328,7 +2200,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C92" t="n">
         <v>1</v>
@@ -2336,11 +2208,7 @@
       <c r="D92" t="n">
         <v>20</v>
       </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
     </row>
     <row r="93">
@@ -2350,7 +2218,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C93" t="n">
         <v>1</v>
@@ -2358,11 +2226,7 @@
       <c r="D93" t="n">
         <v>21</v>
       </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>9, 12, 13</t>
-        </is>
-      </c>
+      <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr"/>
     </row>
     <row r="94">
@@ -2390,7 +2254,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C95" t="n">
         <v>1</v>
@@ -2398,11 +2262,7 @@
       <c r="D95" t="n">
         <v>21</v>
       </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>2, 3, 19</t>
-        </is>
-      </c>
+      <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
     </row>
     <row r="96">
@@ -2430,7 +2290,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C97" t="n">
         <v>2</v>
@@ -2438,11 +2298,7 @@
       <c r="D97" t="n">
         <v>22</v>
       </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>8, 14, 18</t>
-        </is>
-      </c>
+      <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr"/>
     </row>
     <row r="98">
@@ -2470,7 +2326,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C99" t="n">
         <v>2</v>
@@ -2478,11 +2334,7 @@
       <c r="D99" t="n">
         <v>24</v>
       </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>15, 22</t>
-        </is>
-      </c>
+      <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr"/>
     </row>
     <row r="100">
@@ -2492,7 +2344,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C100" t="n">
         <v>1</v>
@@ -2500,11 +2352,7 @@
       <c r="D100" t="n">
         <v>23</v>
       </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>10, 13, 20, 22</t>
-        </is>
-      </c>
+      <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr"/>
     </row>
     <row r="101">
@@ -2532,7 +2380,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C102" t="n">
         <v>1</v>
@@ -2540,11 +2388,7 @@
       <c r="D102" t="n">
         <v>24</v>
       </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>4, 15</t>
-        </is>
-      </c>
+      <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr"/>
     </row>
     <row r="103">
@@ -2554,7 +2398,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C103" t="n">
         <v>1</v>
@@ -2562,11 +2406,7 @@
       <c r="D103" t="n">
         <v>24</v>
       </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>8, 14</t>
-        </is>
-      </c>
+      <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr"/>
     </row>
     <row r="104">
@@ -2576,7 +2416,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C104" t="n">
         <v>1</v>
@@ -2584,11 +2424,7 @@
       <c r="D104" t="n">
         <v>20</v>
       </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>3, 4, 5</t>
-        </is>
-      </c>
+      <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr"/>
     </row>
     <row r="105">
@@ -2598,7 +2434,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C105" t="n">
         <v>1</v>
@@ -2606,11 +2442,7 @@
       <c r="D105" t="n">
         <v>22</v>
       </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>4, 8, 11, 13</t>
-        </is>
-      </c>
+      <c r="E105" t="inlineStr"/>
       <c r="F105" t="inlineStr"/>
     </row>
     <row r="106">
@@ -2638,7 +2470,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C107" t="n">
         <v>1</v>
@@ -2646,11 +2478,7 @@
       <c r="D107" t="n">
         <v>22</v>
       </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>9, 10, 21</t>
-        </is>
-      </c>
+      <c r="E107" t="inlineStr"/>
       <c r="F107" t="inlineStr"/>
     </row>
     <row r="108">
@@ -2660,7 +2488,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C108" t="n">
         <v>2</v>
@@ -2668,11 +2496,7 @@
       <c r="D108" t="n">
         <v>20</v>
       </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
+      <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr"/>
     </row>
     <row r="109">
@@ -2682,7 +2506,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C109" t="n">
         <v>1</v>
@@ -2690,11 +2514,7 @@
       <c r="D109" t="n">
         <v>20</v>
       </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>5, 9, 17</t>
-        </is>
-      </c>
+      <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr"/>
     </row>
     <row r="110">

</xml_diff>

<commit_message>
Added 229 Missing Panel
</commit_message>
<xml_diff>
--- a/reports/missing.xlsx
+++ b/reports/missing.xlsx
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C27" t="n">
         <v>3</v>
@@ -924,7 +924,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>16, 25, 31, 33</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>

</xml_diff>

<commit_message>
updated the missing list
</commit_message>
<xml_diff>
--- a/reports/missing.xlsx
+++ b/reports/missing.xlsx
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C27" t="n">
         <v>3</v>
@@ -922,11 +922,7 @@
       <c r="D27" t="n">
         <v>34</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
@@ -936,7 +932,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C28" t="n">
         <v>2</v>
@@ -944,11 +940,7 @@
       <c r="D28" t="n">
         <v>26</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>8, 11, 15, 19, 21</t>
-        </is>
-      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
@@ -958,7 +950,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C29" t="n">
         <v>1</v>
@@ -966,11 +958,7 @@
       <c r="D29" t="n">
         <v>20</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>3, 6, 13</t>
-        </is>
-      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
@@ -980,7 +968,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
@@ -988,11 +976,7 @@
       <c r="D30" t="n">
         <v>19</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>3, 4, 13</t>
-        </is>
-      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
@@ -1002,7 +986,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C31" t="n">
         <v>1</v>
@@ -1010,11 +994,7 @@
       <c r="D31" t="n">
         <v>28</v>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
@@ -1024,7 +1004,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C32" t="n">
         <v>1</v>
@@ -1032,11 +1012,7 @@
       <c r="D32" t="n">
         <v>23</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
@@ -1046,7 +1022,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C33" t="n">
         <v>1</v>
@@ -1054,11 +1030,7 @@
       <c r="D33" t="n">
         <v>22</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
@@ -1086,7 +1058,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
@@ -1094,11 +1066,7 @@
       <c r="D35" t="n">
         <v>21</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
     </row>
     <row r="36">
@@ -1108,7 +1076,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C36" t="n">
         <v>1</v>
@@ -1116,11 +1084,7 @@
       <c r="D36" t="n">
         <v>19</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>5, 7, 13</t>
-        </is>
-      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
@@ -1130,7 +1094,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C37" t="n">
         <v>1</v>
@@ -1138,11 +1102,7 @@
       <c r="D37" t="n">
         <v>21</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>19, 20</t>
-        </is>
-      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
@@ -1232,7 +1192,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C42" t="n">
         <v>2</v>
@@ -1240,11 +1200,7 @@
       <c r="D42" t="n">
         <v>23</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>4, 8, 11, 22</t>
-        </is>
-      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
@@ -1254,7 +1210,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C43" t="n">
         <v>1</v>
@@ -1262,11 +1218,7 @@
       <c r="D43" t="n">
         <v>22</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>9, 10, 12, 16, 19</t>
-        </is>
-      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
@@ -1276,7 +1228,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C44" t="n">
         <v>1</v>
@@ -1284,11 +1236,7 @@
       <c r="D44" t="n">
         <v>21</v>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
@@ -1298,7 +1246,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C45" t="n">
         <v>1</v>
@@ -1306,11 +1254,7 @@
       <c r="D45" t="n">
         <v>23</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
@@ -1320,7 +1264,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C46" t="n">
         <v>1</v>
@@ -1328,11 +1272,7 @@
       <c r="D46" t="n">
         <v>22</v>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>9, 11</t>
-        </is>
-      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
@@ -1342,7 +1282,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C47" t="n">
         <v>1</v>
@@ -1350,11 +1290,7 @@
       <c r="D47" t="n">
         <v>23</v>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>6, 16</t>
-        </is>
-      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
@@ -1364,7 +1300,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C48" t="n">
         <v>1</v>
@@ -1372,11 +1308,7 @@
       <c r="D48" t="n">
         <v>19</v>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>6, 17</t>
-        </is>
-      </c>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
@@ -1386,7 +1318,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C49" t="n">
         <v>1</v>
@@ -1394,11 +1326,7 @@
       <c r="D49" t="n">
         <v>21</v>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>8, 17</t>
-        </is>
-      </c>
+      <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
@@ -1408,7 +1336,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C50" t="n">
         <v>1</v>
@@ -1416,11 +1344,7 @@
       <c r="D50" t="n">
         <v>22</v>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>3, 8, 10, 11, 17</t>
-        </is>
-      </c>
+      <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
@@ -1430,7 +1354,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C51" t="n">
         <v>1</v>
@@ -1438,11 +1362,7 @@
       <c r="D51" t="n">
         <v>22</v>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
+      <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
     </row>
     <row r="52">
@@ -1470,7 +1390,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C53" t="n">
         <v>1</v>
@@ -1478,11 +1398,7 @@
       <c r="D53" t="n">
         <v>20</v>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
@@ -1510,7 +1426,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C55" t="n">
         <v>1</v>
@@ -1518,11 +1434,7 @@
       <c r="D55" t="n">
         <v>26</v>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>14, 16, 21, 23</t>
-        </is>
-      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
@@ -1532,7 +1444,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C56" t="n">
         <v>1</v>
@@ -1540,11 +1452,7 @@
       <c r="D56" t="n">
         <v>19</v>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>2, 6</t>
-        </is>
-      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
@@ -1554,7 +1462,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C57" t="n">
         <v>1</v>
@@ -1562,11 +1470,7 @@
       <c r="D57" t="n">
         <v>22</v>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>2, 3, 4, 11, 14, 18</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
     </row>
     <row r="58">
@@ -1576,7 +1480,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C58" t="n">
         <v>1</v>
@@ -1584,11 +1488,7 @@
       <c r="D58" t="n">
         <v>23</v>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>2, 13, 14, 16, 17</t>
-        </is>
-      </c>
+      <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
@@ -1598,7 +1498,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C59" t="n">
         <v>1</v>
@@ -1606,11 +1506,7 @@
       <c r="D59" t="n">
         <v>22</v>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>5, 14, 21</t>
-        </is>
-      </c>
+      <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
@@ -1620,7 +1516,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C60" t="n">
         <v>1</v>
@@ -1628,11 +1524,7 @@
       <c r="D60" t="n">
         <v>26</v>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>5, 7</t>
-        </is>
-      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
     </row>
     <row r="61">
@@ -2524,7 +2416,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C110" t="n">
         <v>1</v>
@@ -2532,11 +2424,7 @@
       <c r="D110" t="n">
         <v>19</v>
       </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>5, 6, 13</t>
-        </is>
-      </c>
+      <c r="E110" t="inlineStr"/>
       <c r="F110" t="inlineStr"/>
     </row>
     <row r="111">
@@ -2546,7 +2434,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C111" t="n">
         <v>1</v>
@@ -2554,11 +2442,7 @@
       <c r="D111" t="n">
         <v>24</v>
       </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>10, 17</t>
-        </is>
-      </c>
+      <c r="E111" t="inlineStr"/>
       <c r="F111" t="inlineStr"/>
     </row>
     <row r="112">
@@ -2568,7 +2452,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C112" t="n">
         <v>1</v>
@@ -2576,11 +2460,7 @@
       <c r="D112" t="n">
         <v>23</v>
       </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>4, 7, 11, 15, 17</t>
-        </is>
-      </c>
+      <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr"/>
     </row>
     <row r="113">
@@ -2590,7 +2470,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C113" t="n">
         <v>1</v>
@@ -2598,11 +2478,7 @@
       <c r="D113" t="n">
         <v>20</v>
       </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>7, 15</t>
-        </is>
-      </c>
+      <c r="E113" t="inlineStr"/>
       <c r="F113" t="inlineStr"/>
     </row>
     <row r="114">
@@ -2630,7 +2506,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C115" t="n">
         <v>1</v>
@@ -2638,11 +2514,7 @@
       <c r="D115" t="n">
         <v>20</v>
       </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>4, 8, 9, 17, 19</t>
-        </is>
-      </c>
+      <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
     </row>
     <row r="116">
@@ -2652,7 +2524,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C116" t="n">
         <v>1</v>
@@ -2660,11 +2532,7 @@
       <c r="D116" t="n">
         <v>22</v>
       </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>2, 15, 16, 17, 19, 21</t>
-        </is>
-      </c>
+      <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
     </row>
     <row r="117">
@@ -2674,7 +2542,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C117" t="n">
         <v>1</v>
@@ -2682,11 +2550,7 @@
       <c r="D117" t="n">
         <v>20</v>
       </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr"/>
     </row>
     <row r="118">
@@ -2696,7 +2560,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C118" t="n">
         <v>1</v>
@@ -2704,11 +2568,7 @@
       <c r="D118" t="n">
         <v>22</v>
       </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>7, 15, 16, 20</t>
-        </is>
-      </c>
+      <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
     </row>
     <row r="119">
@@ -2718,7 +2578,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C119" t="n">
         <v>1</v>
@@ -2726,11 +2586,7 @@
       <c r="D119" t="n">
         <v>23</v>
       </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>15, 17</t>
-        </is>
-      </c>
+      <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
     </row>
     <row r="120">
@@ -2740,7 +2596,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C120" t="n">
         <v>2</v>
@@ -2748,11 +2604,7 @@
       <c r="D120" t="n">
         <v>24</v>
       </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>7, 11, 17</t>
-        </is>
-      </c>
+      <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
     </row>
     <row r="121">
@@ -2762,7 +2614,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C121" t="n">
         <v>1</v>
@@ -2770,11 +2622,7 @@
       <c r="D121" t="n">
         <v>23</v>
       </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>2, 4, 16</t>
-        </is>
-      </c>
+      <c r="E121" t="inlineStr"/>
       <c r="F121" t="inlineStr"/>
     </row>
     <row r="122">
@@ -2784,7 +2632,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C122" t="n">
         <v>2</v>
@@ -2792,11 +2640,7 @@
       <c r="D122" t="n">
         <v>22</v>
       </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>5, 8, 9, 15, 17, 19</t>
-        </is>
-      </c>
+      <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr"/>
     </row>
     <row r="123">
@@ -2806,7 +2650,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C123" t="n">
         <v>1</v>
@@ -2814,11 +2658,7 @@
       <c r="D123" t="n">
         <v>22</v>
       </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>6, 13, 17, 18, 20</t>
-        </is>
-      </c>
+      <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
     </row>
     <row r="124">
@@ -2828,7 +2668,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C124" t="n">
         <v>1</v>
@@ -2836,11 +2676,7 @@
       <c r="D124" t="n">
         <v>20</v>
       </c>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>2, 4, 7, 11, 13</t>
-        </is>
-      </c>
+      <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
     </row>
     <row r="125">
@@ -2850,7 +2686,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C125" t="n">
         <v>1</v>
@@ -2858,11 +2694,7 @@
       <c r="D125" t="n">
         <v>22</v>
       </c>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
+      <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
     </row>
     <row r="126">
@@ -2872,7 +2704,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C126" t="n">
         <v>1</v>
@@ -2880,11 +2712,7 @@
       <c r="D126" t="n">
         <v>18</v>
       </c>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>3, 12, 16</t>
-        </is>
-      </c>
+      <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
     </row>
     <row r="127">
@@ -2894,7 +2722,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C127" t="n">
         <v>2</v>
@@ -2902,11 +2730,7 @@
       <c r="D127" t="n">
         <v>22</v>
       </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>5, 12</t>
-        </is>
-      </c>
+      <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
     </row>
     <row r="128">
@@ -2916,7 +2740,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C128" t="n">
         <v>2</v>
@@ -2924,11 +2748,7 @@
       <c r="D128" t="n">
         <v>16</v>
       </c>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+      <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
     </row>
     <row r="129">
@@ -2938,7 +2758,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C129" t="n">
         <v>2</v>
@@ -2946,11 +2766,7 @@
       <c r="D129" t="n">
         <v>18</v>
       </c>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>9, 10, 13</t>
-        </is>
-      </c>
+      <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
     </row>
     <row r="130">
@@ -2960,7 +2776,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C130" t="n">
         <v>1</v>
@@ -2968,11 +2784,7 @@
       <c r="D130" t="n">
         <v>20</v>
       </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>5, 9, 11, 13, 14</t>
-        </is>
-      </c>
+      <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
     </row>
     <row r="131">
@@ -2982,7 +2794,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C131" t="n">
         <v>3</v>
@@ -2990,11 +2802,7 @@
       <c r="D131" t="n">
         <v>18</v>
       </c>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>5, 6, 8, 15, 16</t>
-        </is>
-      </c>
+      <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
     </row>
     <row r="132">
@@ -3004,7 +2812,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C132" t="n">
         <v>1</v>
@@ -3012,11 +2820,7 @@
       <c r="D132" t="n">
         <v>23</v>
       </c>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>5, 6, 7, 10, 14, 18</t>
-        </is>
-      </c>
+      <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
     </row>
     <row r="133">
@@ -3026,7 +2830,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C133" t="n">
         <v>2</v>
@@ -3034,11 +2838,7 @@
       <c r="D133" t="n">
         <v>23</v>
       </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>5, 17, 19</t>
-        </is>
-      </c>
+      <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
     </row>
     <row r="134">
@@ -3048,7 +2848,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C134" t="n">
         <v>2</v>
@@ -3056,11 +2856,7 @@
       <c r="D134" t="n">
         <v>24</v>
       </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>7, 14, 16, 19, 23</t>
-        </is>
-      </c>
+      <c r="E134" t="inlineStr"/>
       <c r="F134" t="inlineStr"/>
     </row>
     <row r="135">
@@ -3070,7 +2866,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C135" t="n">
         <v>1</v>
@@ -3078,11 +2874,7 @@
       <c r="D135" t="n">
         <v>21</v>
       </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>4, 7, 8, 15, 19</t>
-        </is>
-      </c>
+      <c r="E135" t="inlineStr"/>
       <c r="F135" t="inlineStr"/>
     </row>
     <row r="136">
@@ -3092,7 +2884,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C136" t="n">
         <v>2</v>
@@ -3100,11 +2892,7 @@
       <c r="D136" t="n">
         <v>22</v>
       </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>7, 11, 12, 17, 21</t>
-        </is>
-      </c>
+      <c r="E136" t="inlineStr"/>
       <c r="F136" t="inlineStr"/>
     </row>
     <row r="137">
@@ -3114,7 +2902,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C137" t="n">
         <v>1</v>
@@ -3122,11 +2910,7 @@
       <c r="D137" t="n">
         <v>21</v>
       </c>
-      <c r="E137" t="inlineStr">
-        <is>
-          <t>3, 7, 8, 10, 17</t>
-        </is>
-      </c>
+      <c r="E137" t="inlineStr"/>
       <c r="F137" t="inlineStr"/>
     </row>
     <row r="138">
@@ -3136,7 +2920,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C138" t="n">
         <v>2</v>
@@ -3144,11 +2928,7 @@
       <c r="D138" t="n">
         <v>26</v>
       </c>
-      <c r="E138" t="inlineStr">
-        <is>
-          <t>13, 18, 19, 20</t>
-        </is>
-      </c>
+      <c r="E138" t="inlineStr"/>
       <c r="F138" t="inlineStr"/>
     </row>
     <row r="139">
@@ -3158,7 +2938,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C139" t="n">
         <v>1</v>
@@ -3166,11 +2946,7 @@
       <c r="D139" t="n">
         <v>23</v>
       </c>
-      <c r="E139" t="inlineStr">
-        <is>
-          <t>5, 14</t>
-        </is>
-      </c>
+      <c r="E139" t="inlineStr"/>
       <c r="F139" t="inlineStr"/>
     </row>
     <row r="140">
@@ -3180,7 +2956,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C140" t="n">
         <v>1</v>
@@ -3188,11 +2964,7 @@
       <c r="D140" t="n">
         <v>21</v>
       </c>
-      <c r="E140" t="inlineStr">
-        <is>
-          <t>2, 12, 16, 17</t>
-        </is>
-      </c>
+      <c r="E140" t="inlineStr"/>
       <c r="F140" t="inlineStr"/>
     </row>
     <row r="141">
@@ -3202,7 +2974,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C141" t="n">
         <v>1</v>
@@ -3210,11 +2982,7 @@
       <c r="D141" t="n">
         <v>20</v>
       </c>
-      <c r="E141" t="inlineStr">
-        <is>
-          <t>12, 16, 17, 18</t>
-        </is>
-      </c>
+      <c r="E141" t="inlineStr"/>
       <c r="F141" t="inlineStr"/>
     </row>
     <row r="142">
@@ -3224,7 +2992,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C142" t="n">
         <v>1</v>
@@ -3232,11 +3000,7 @@
       <c r="D142" t="n">
         <v>21</v>
       </c>
-      <c r="E142" t="inlineStr">
-        <is>
-          <t>2, 3, 12, 14, 16, 18, 19</t>
-        </is>
-      </c>
+      <c r="E142" t="inlineStr"/>
       <c r="F142" t="inlineStr"/>
     </row>
     <row r="143">
@@ -3246,7 +3010,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C143" t="n">
         <v>1</v>
@@ -3254,11 +3018,7 @@
       <c r="D143" t="n">
         <v>18</v>
       </c>
-      <c r="E143" t="inlineStr">
-        <is>
-          <t>8, 14, 15</t>
-        </is>
-      </c>
+      <c r="E143" t="inlineStr"/>
       <c r="F143" t="inlineStr"/>
     </row>
     <row r="144">
@@ -3268,7 +3028,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C144" t="n">
         <v>1</v>
@@ -3276,11 +3036,7 @@
       <c r="D144" t="n">
         <v>23</v>
       </c>
-      <c r="E144" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
+      <c r="E144" t="inlineStr"/>
       <c r="F144" t="inlineStr"/>
     </row>
     <row r="145">
@@ -3290,7 +3046,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C145" t="n">
         <v>1</v>
@@ -3298,11 +3054,7 @@
       <c r="D145" t="n">
         <v>24</v>
       </c>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
+      <c r="E145" t="inlineStr"/>
       <c r="F145" t="inlineStr"/>
     </row>
     <row r="146">
@@ -3330,7 +3082,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C147" t="n">
         <v>1</v>
@@ -3338,11 +3090,7 @@
       <c r="D147" t="n">
         <v>22</v>
       </c>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t>6, 9, 13</t>
-        </is>
-      </c>
+      <c r="E147" t="inlineStr"/>
       <c r="F147" t="inlineStr"/>
     </row>
     <row r="148">
@@ -3352,7 +3100,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C148" t="n">
         <v>1</v>
@@ -3360,11 +3108,7 @@
       <c r="D148" t="n">
         <v>23</v>
       </c>
-      <c r="E148" t="inlineStr">
-        <is>
-          <t>6, 17</t>
-        </is>
-      </c>
+      <c r="E148" t="inlineStr"/>
       <c r="F148" t="inlineStr"/>
     </row>
     <row r="149">
@@ -3374,7 +3118,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C149" t="n">
         <v>1</v>
@@ -3382,11 +3126,7 @@
       <c r="D149" t="n">
         <v>22</v>
       </c>
-      <c r="E149" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
+      <c r="E149" t="inlineStr"/>
       <c r="F149" t="inlineStr"/>
     </row>
     <row r="150">
@@ -3396,7 +3136,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C150" t="n">
         <v>1</v>
@@ -3404,11 +3144,7 @@
       <c r="D150" t="n">
         <v>20</v>
       </c>
-      <c r="E150" t="inlineStr">
-        <is>
-          <t>3, 10, 17, 19</t>
-        </is>
-      </c>
+      <c r="E150" t="inlineStr"/>
       <c r="F150" t="inlineStr"/>
     </row>
     <row r="151">
@@ -3418,7 +3154,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C151" t="n">
         <v>1</v>
@@ -3426,11 +3162,7 @@
       <c r="D151" t="n">
         <v>22</v>
       </c>
-      <c r="E151" t="inlineStr">
-        <is>
-          <t>4, 16, 21</t>
-        </is>
-      </c>
+      <c r="E151" t="inlineStr"/>
       <c r="F151" t="inlineStr"/>
     </row>
     <row r="152">
@@ -3440,7 +3172,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C152" t="n">
         <v>1</v>
@@ -3448,11 +3180,7 @@
       <c r="D152" t="n">
         <v>20</v>
       </c>
-      <c r="E152" t="inlineStr">
-        <is>
-          <t>13, 14, 15</t>
-        </is>
-      </c>
+      <c r="E152" t="inlineStr"/>
       <c r="F152" t="inlineStr"/>
     </row>
     <row r="153">
@@ -3480,7 +3208,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C154" t="n">
         <v>1</v>
@@ -3488,11 +3216,7 @@
       <c r="D154" t="n">
         <v>21</v>
       </c>
-      <c r="E154" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
+      <c r="E154" t="inlineStr"/>
       <c r="F154" t="inlineStr"/>
     </row>
     <row r="155">
@@ -3538,7 +3262,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C157" t="n">
         <v>1</v>
@@ -3546,11 +3270,7 @@
       <c r="D157" t="n">
         <v>20</v>
       </c>
-      <c r="E157" t="inlineStr">
-        <is>
-          <t>9, 11</t>
-        </is>
-      </c>
+      <c r="E157" t="inlineStr"/>
       <c r="F157" t="inlineStr"/>
     </row>
     <row r="158">
@@ -3662,7 +3382,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C163" t="n">
         <v>1</v>
@@ -3670,11 +3390,7 @@
       <c r="D163" t="n">
         <v>22</v>
       </c>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
+      <c r="E163" t="inlineStr"/>
       <c r="F163" t="inlineStr"/>
     </row>
     <row r="164">
@@ -3702,7 +3418,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C165" t="n">
         <v>1</v>
@@ -3710,11 +3426,7 @@
       <c r="D165" t="n">
         <v>22</v>
       </c>
-      <c r="E165" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
+      <c r="E165" t="inlineStr"/>
       <c r="F165" t="inlineStr"/>
     </row>
     <row r="166">
@@ -3724,7 +3436,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C166" t="n">
         <v>1</v>
@@ -3732,11 +3444,7 @@
       <c r="D166" t="n">
         <v>20</v>
       </c>
-      <c r="E166" t="inlineStr">
-        <is>
-          <t>5, 16</t>
-        </is>
-      </c>
+      <c r="E166" t="inlineStr"/>
       <c r="F166" t="inlineStr"/>
     </row>
     <row r="167">
@@ -3746,7 +3454,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C167" t="n">
         <v>2</v>
@@ -3754,11 +3462,7 @@
       <c r="D167" t="n">
         <v>22</v>
       </c>
-      <c r="E167" t="inlineStr">
-        <is>
-          <t>14, 21</t>
-        </is>
-      </c>
+      <c r="E167" t="inlineStr"/>
       <c r="F167" t="inlineStr"/>
     </row>
     <row r="168">
@@ -3768,7 +3472,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C168" t="n">
         <v>1</v>
@@ -3776,11 +3480,7 @@
       <c r="D168" t="n">
         <v>23</v>
       </c>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>13, 16</t>
-        </is>
-      </c>
+      <c r="E168" t="inlineStr"/>
       <c r="F168" t="inlineStr"/>
     </row>
     <row r="169">
@@ -3790,7 +3490,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C169" t="n">
         <v>1</v>
@@ -3798,11 +3498,7 @@
       <c r="D169" t="n">
         <v>24</v>
       </c>
-      <c r="E169" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="E169" t="inlineStr"/>
       <c r="F169" t="inlineStr"/>
     </row>
     <row r="170">
@@ -3830,7 +3526,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C171" t="n">
         <v>1</v>
@@ -3838,11 +3534,7 @@
       <c r="D171" t="n">
         <v>20</v>
       </c>
-      <c r="E171" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
+      <c r="E171" t="inlineStr"/>
       <c r="F171" t="inlineStr"/>
     </row>
     <row r="172">
@@ -3852,7 +3544,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C172" t="n">
         <v>1</v>
@@ -3860,11 +3552,7 @@
       <c r="D172" t="n">
         <v>23</v>
       </c>
-      <c r="E172" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
+      <c r="E172" t="inlineStr"/>
       <c r="F172" t="inlineStr"/>
     </row>
     <row r="173">
@@ -3874,7 +3562,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C173" t="n">
         <v>1</v>
@@ -3882,11 +3570,7 @@
       <c r="D173" t="n">
         <v>23</v>
       </c>
-      <c r="E173" t="inlineStr">
-        <is>
-          <t>14, 17, 22</t>
-        </is>
-      </c>
+      <c r="E173" t="inlineStr"/>
       <c r="F173" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>